<commit_message>
Convert to 7 bit
</commit_message>
<xml_diff>
--- a/RversusVout.xlsx
+++ b/RversusVout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrp2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrp2/Documents/GitHub/arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AE8825B-202B-B846-ABB4-DF274735FDAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400F37D8-39CA-0C42-AEF4-339C9DFB42D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F794C043-F984-E241-8DB7-3265841CE459}"/>
   </bookViews>
@@ -109,7 +109,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Permanent R at 48V =  70K
+          <t xml:space="preserve">Permanent R at 48V =  70K.........R network starts at 47K, so Rperm = 23K.
 </t>
         </r>
         <r>
@@ -119,7 +119,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Permanent R at 36V =  44K
+          <t xml:space="preserve">Permanent R at 36V =  44K ....... R network starts at 47K , so Rperm = 0 .
 </t>
         </r>
         <r>
@@ -148,12 +148,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Voltage</t>
   </si>
   <si>
     <t>Resistance</t>
+  </si>
+  <si>
+    <t>7 bit values :</t>
   </si>
 </sst>
 </file>
@@ -1298,6 +1301,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>59070</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561164</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129423</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{796BAE04-89D1-224E-9D68-C1EE863F290C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14590233" y="2451395"/>
+          <a:ext cx="5463954" cy="2639888"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1598,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542E829E-12AC-DF4E-A1DC-283E8DA0FF33}">
-  <dimension ref="B1:G11"/>
+  <dimension ref="B1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1610,63 +1657,90 @@
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="Q1">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>27.7</v>
       </c>
       <c r="C2">
         <v>45800</v>
       </c>
+      <c r="Q2">
+        <f>Q1/2</f>
+        <v>12500</v>
+      </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>32.1</v>
       </c>
       <c r="C3">
         <v>55400</v>
       </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q7" si="0">Q2/2</f>
+        <v>6250</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>37.200000000000003</v>
       </c>
       <c r="C4">
         <v>65900</v>
       </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>3125</v>
+      </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>41.8</v>
       </c>
       <c r="C5">
         <v>76700</v>
       </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>1562.5</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>46.2</v>
       </c>
       <c r="C6">
         <v>86400</v>
       </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>781.25</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>48.2</v>
       </c>
       <c r="C7">
         <v>91600</v>
       </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>390.625</v>
+      </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>52.9</v>
       </c>
@@ -1674,7 +1748,7 @@
         <v>101000</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>57</v>
       </c>
@@ -1682,15 +1756,18 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>57.7</v>
       </c>
       <c r="C10">
         <v>112000</v>
       </c>
+      <c r="T10" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>69.2</v>
       </c>

</xml_diff>